<commit_message>
Redone the shit, cause it screwed up.
</commit_message>
<xml_diff>
--- a/docs/meten-aan-de-robot/meetresultaten/EPO2_meetresultaten_robot_joris_chy.xlsx
+++ b/docs/meten-aan-de-robot/meetresultaten/EPO2_meetresultaten_robot_joris_chy.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="28620" windowHeight="12660"/>
@@ -11,7 +11,7 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -45,11 +45,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,7 +98,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -106,11 +106,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -184,6 +189,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -218,6 +224,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -393,14 +400,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -409,7 +416,7 @@
     <col min="5" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
@@ -432,7 +439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1.1280920000000001</v>
       </c>
@@ -455,7 +462,7 @@
         <v>2.8595009999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1.1266860000000001</v>
       </c>
@@ -478,7 +485,7 @@
         <v>2.8563749999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1.136819</v>
       </c>
@@ -501,7 +508,7 @@
         <v>2.8452099999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1.1421840000000001</v>
       </c>
@@ -524,7 +531,7 @@
         <v>2.8501050000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1.1302989999999999</v>
       </c>
@@ -547,7 +554,7 @@
         <v>2.859677</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1.1360319999999999</v>
       </c>
@@ -555,7 +562,7 @@
         <v>2.6826650000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1.1403810000000001</v>
       </c>
@@ -563,7 +570,7 @@
         <v>2.6662189999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>1.130258</v>
       </c>
@@ -571,7 +578,7 @@
         <v>2.6645029999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1.131067</v>
       </c>
@@ -579,7 +586,7 @@
         <v>2.6505640000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>1.1446160000000001</v>
       </c>
@@ -592,7 +599,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1">
+    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
@@ -632,24 +639,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>